<commit_message>
fixed c++ block implementation
</commit_message>
<xml_diff>
--- a/Measurement/C++ Performance Measurement.xlsx
+++ b/Measurement/C++ Performance Measurement.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813E37EB-254A-484D-A3E2-52F83F1DF08B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58468C01-DAA6-48B4-B6FB-51F00B29A022}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Data Size</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>10K</t>
+  </si>
+  <si>
+    <t>Block Size\Data Size</t>
   </si>
 </sst>
 </file>
@@ -639,7 +642,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,12 +837,18 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -857,16 +866,49 @@
       <c r="A2">
         <v>128</v>
       </c>
+      <c r="B2">
+        <v>26.37</v>
+      </c>
+      <c r="C2">
+        <v>87.391000000000005</v>
+      </c>
+      <c r="D2">
+        <v>209.76599999999999</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>256</v>
       </c>
+      <c r="B3">
+        <v>24.9</v>
+      </c>
+      <c r="C3">
+        <v>87.281000000000006</v>
+      </c>
+      <c r="D3">
+        <v>211.23400000000001</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>512</v>
       </c>
+      <c r="B4">
+        <v>20.655999999999999</v>
+      </c>
+      <c r="C4">
+        <v>75.796999999999997</v>
+      </c>
+      <c r="D4">
+        <v>190.40600000000001</v>
+      </c>
+      <c r="E4">
+        <v>380.34399999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D5" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E12" s="1"/>
@@ -876,5 +918,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>